<commit_message>
Add economy totals/earnings by ed level to basic table
</commit_message>
<xml_diff>
--- a/deliverables/males_underemployed_2010-2012.xlsx
+++ b/deliverables/males_underemployed_2010-2012.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>status</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>grad_lf_status</t>
+  </si>
+  <si>
+    <t>Economy Total</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -215,8 +218,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -226,8 +266,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -241,14 +285,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -263,25 +299,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -611,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N17"/>
+  <dimension ref="A2:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -625,22 +671,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="25" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="27"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -649,600 +695,642 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30">
+        <v>23779011</v>
+      </c>
+      <c r="D4" s="31">
+        <v>64604176</v>
+      </c>
+      <c r="E4" s="31">
+        <v>39715710</v>
+      </c>
+      <c r="F4" s="31">
+        <v>19156372</v>
+      </c>
+      <c r="G4" s="31">
+        <v>46438460</v>
+      </c>
+      <c r="H4" s="32">
+        <v>25359154</v>
+      </c>
+      <c r="I4" s="33">
+        <v>17536</v>
+      </c>
+      <c r="J4" s="34">
+        <v>30409</v>
+      </c>
+      <c r="K4" s="34">
+        <v>31978</v>
+      </c>
+      <c r="L4" s="34">
+        <v>41943</v>
+      </c>
+      <c r="M4" s="34">
+        <v>55000</v>
+      </c>
+      <c r="N4" s="35">
+        <v>78397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C5" s="1">
         <v>21796149</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D5" s="2">
         <v>52674853</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E5" s="2">
         <v>26899556</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F5" s="2">
         <v>11699028</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G5" s="21">
         <v>12147583</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H5" s="3">
         <v>2139562</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I5" s="7">
         <v>17165</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J5" s="8">
         <v>28311</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K5" s="8">
         <v>27000</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L5" s="8">
         <v>36600</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M5" s="24">
         <v>36000</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N5" s="9">
         <v>34000</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>65842</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>576427</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>766133</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>416948</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G6" s="21">
         <v>2954642</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H6" s="3">
         <v>5944479</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I6" s="7">
         <v>51577</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J6" s="8">
         <v>62914</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K6" s="8">
         <v>64987</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L6" s="8">
         <v>73400</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M6" s="24">
         <v>85983</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N6" s="9">
         <v>99614</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22" t="s">
+    <row r="7" spans="1:14">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>1917019</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>11352896</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>12050021</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>7040396</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G7" s="21">
         <v>31336235</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H7" s="3">
         <v>17275114</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I7" s="7">
         <v>21456</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J7" s="8">
         <v>41419</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K7" s="8">
         <v>45000</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L7" s="8">
         <v>51577</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M7" s="24">
         <v>62914</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N7" s="9">
         <v>78643</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="21" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>20640357</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>51907839</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>29016771</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>13413646</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>21004785</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H8" s="22">
         <v>4877726</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I8" s="7">
         <v>17000</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J8" s="8">
         <v>28311</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K8" s="8">
         <v>28311</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L8" s="8">
         <v>38500</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M8" s="8">
         <v>47000</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N8" s="25">
         <v>52000</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>3138653</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>12696337</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>10698939</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>5742727</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>25433675</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H9" s="22">
         <v>20481428</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I9" s="7">
         <v>20631</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J9" s="8">
         <v>41262</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K9" s="8">
         <v>46000</v>
-      </c>
-      <c r="L8" s="8">
-        <v>51577</v>
-      </c>
-      <c r="M8" s="8">
-        <v>62600</v>
-      </c>
-      <c r="N8" s="35">
-        <v>82523</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>325133</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2061411</v>
-      </c>
-      <c r="E9" s="30">
-        <v>3054991</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2255225</v>
-      </c>
-      <c r="G9" s="2">
-        <v>12497510</v>
-      </c>
-      <c r="H9" s="37">
-        <v>13114348</v>
-      </c>
-      <c r="I9" s="7">
-        <v>15473</v>
-      </c>
-      <c r="J9" s="8">
-        <v>37749</v>
-      </c>
-      <c r="K9" s="34">
-        <v>37136</v>
       </c>
       <c r="L9" s="8">
         <v>51577</v>
       </c>
       <c r="M9" s="8">
+        <v>62600</v>
+      </c>
+      <c r="N9" s="25">
+        <v>82523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>325133</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2061411</v>
+      </c>
+      <c r="E10" s="21">
+        <v>3054991</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2255225</v>
+      </c>
+      <c r="G10" s="2">
+        <v>12497510</v>
+      </c>
+      <c r="H10" s="27">
+        <v>13114348</v>
+      </c>
+      <c r="I10" s="7">
+        <v>15473</v>
+      </c>
+      <c r="J10" s="8">
+        <v>37749</v>
+      </c>
+      <c r="K10" s="24">
+        <v>37136</v>
+      </c>
+      <c r="L10" s="8">
+        <v>51577</v>
+      </c>
+      <c r="M10" s="8">
         <v>60000</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N10" s="9">
         <v>80000</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22" t="s">
+    <row r="11" spans="1:14">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>494464</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>4064004</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E11" s="21">
         <v>3936035</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>1970003</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <v>10591802</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H11" s="3">
         <v>4843201</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I11" s="7">
         <v>26214</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J11" s="8">
         <v>47186</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K11" s="24">
         <v>51577</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L11" s="8">
         <v>52000</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M11" s="8">
         <v>72351</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N11" s="9">
         <v>92839</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22" t="s">
+    <row r="12" spans="1:14">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>22959414</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>58478761</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E12" s="21">
         <v>32724684</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>14931145</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>23349148</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H12" s="3">
         <v>7401605</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I12" s="7">
         <v>17536</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J12" s="8">
         <v>29925</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K12" s="24">
         <v>30000</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L12" s="8">
         <v>40000</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M12" s="8">
         <v>47186</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N12" s="9">
         <v>65000</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="21" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>14479442</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D13" s="21">
         <v>22948224</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E13" s="2">
         <v>10989025</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>4297559</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <v>4800585</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H13" s="3">
         <v>2302569</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I13" s="7">
         <v>14680</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J13" s="24">
         <v>20012</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K13" s="8">
         <v>16500</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L13" s="8">
         <v>27852</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M13" s="8">
         <v>28883</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N13" s="9">
         <v>50096</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>158774</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D14" s="21">
         <v>663080</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <v>1105930</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <v>581324</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <v>4711663</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H14" s="3">
         <v>6069189</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I14" s="7">
         <v>13823</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J14" s="24">
         <v>30946</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K14" s="8">
         <v>48000</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L14" s="8">
         <v>50437</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M14" s="8">
         <v>51577</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N14" s="9">
         <v>75000</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>9140794</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D15" s="21">
         <v>40992872</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="2">
         <v>27620754</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="2">
         <v>14277490</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="2">
         <v>36926212</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>16987396</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I15" s="7">
         <v>24633</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J15" s="24">
         <v>37000</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K15" s="8">
         <v>39846</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L15" s="8">
         <v>46419</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M15" s="8">
         <v>60000</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N15" s="9">
         <v>82523</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="21" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>23779011</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <v>64604176</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>39715710</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F16" s="21">
         <v>2255225</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>46438460</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <v>25359154</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I16" s="7">
         <v>17536</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J16" s="8">
         <v>30409</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K16" s="8">
         <v>31978</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L16" s="24">
         <v>51577</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M16" s="8">
         <v>55000</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N16" s="9">
         <v>78397</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22" t="s">
+    <row r="17" spans="1:14">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="30">
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="21">
         <v>1970003</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="34">
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="24">
         <v>52000</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24" t="s">
+      <c r="M17" s="8"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="32">
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="23">
         <v>14931145</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="36">
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="26">
         <v>40000</v>
       </c>
-      <c r="M17" s="11"/>
-      <c r="N17" s="12"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>